<commit_message>
Error search matrix definition both for Hydon and DBH
</commit_message>
<xml_diff>
--- a/Input/linear_model.xlsx
+++ b/Input/linear_model.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">Model name</t>
   </si>
@@ -46,25 +46,10 @@
     <t xml:space="preserve">u</t>
   </si>
   <si>
-    <t xml:space="preserve">a(t)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a(t)*u+b(t)*v</t>
+    <t xml:space="preserve">u+v</t>
   </si>
   <si>
     <t xml:space="preserve">v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b(t)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c(t)*u+d(t)*v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c(t)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d(t)</t>
   </si>
 </sst>
 </file>
@@ -79,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,10 +153,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.21"/>
   </cols>
@@ -202,38 +188,29 @@
       <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>